<commit_message>
Updated gyros, accelerometers, budget
Still not sure about a lot of specs, but maybe this is enough for the
techfair app at this point. I updated the app, too.
</commit_message>
<xml_diff>
--- a/budget.xlsx
+++ b/budget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\Desktop\pixel-props\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>comments</t>
   </si>
@@ -48,15 +47,6 @@
     <t>tubes</t>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>controllers</t>
-  </si>
-  <si>
-    <t>misc power / control circuitry</t>
-  </si>
-  <si>
     <t>accelerometer</t>
   </si>
   <si>
@@ -72,20 +62,57 @@
     <t>wireless communications</t>
   </si>
   <si>
-    <t>Final</t>
-  </si>
-  <si>
-    <t>Prototype</t>
-  </si>
-  <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>controller / amp stuff for LEDs</t>
+  </si>
+  <si>
+    <t>final product quantity</t>
+  </si>
+  <si>
+    <t>quantity for prototyping</t>
+  </si>
+  <si>
+    <t>microcontroller</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>price ea</t>
+  </si>
+  <si>
+    <t>other hardware, leashes</t>
+  </si>
+  <si>
+    <t>ftdi thing</t>
+  </si>
+  <si>
+    <t>guessing on price</t>
+  </si>
+  <si>
+    <t>misc circuitry (power? other?)</t>
+  </si>
+  <si>
+    <t>cost of producing boards?</t>
+  </si>
+  <si>
+    <t>any tools for prototyping?</t>
+  </si>
+  <si>
+    <t>Item</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +124,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -119,15 +153,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -407,132 +448,254 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D1" t="s">
+    <row r="1" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="3">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>C5*2</f>
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3">
+        <f>D5*(C5+B5)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>C6*2</f>
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3">
+        <f>D6*(C6+B6)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B7">
+        <f>C7</f>
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3">
+        <f>D7*(C7+B7)</f>
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="3">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>30</v>
+      </c>
+      <c r="E10" s="3">
+        <f>D10*(C10+B10)</f>
+        <v>60</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3">
+        <f>D11*(C11+B11)</f>
+        <v>4</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="3">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="3">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>100</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="3">
         <v>10</v>
       </c>
-      <c r="C7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>12</v>
       </c>
-      <c r="C9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <f>2*4+4</f>
-        <v>12</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20">
-        <f>SUM(C4:C19)</f>
-        <v>217</v>
-      </c>
+      <c r="E18" s="3">
+        <f>SUM(E2:E16)</f>
+        <v>370</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1"/>
+    <hyperlink ref="F11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>